<commit_message>
fixed task 10 graph
</commit_message>
<xml_diff>
--- a/10-13 tezni-bernoullijeva/prosti pad.xlsx
+++ b/10-13 tezni-bernoullijeva/prosti pad.xlsx
@@ -1,31 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\archW\Desktop\fizikalni-praktikum\meritve vaja 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\archW\Desktop\faks\fizikalni-praktikum\10-13 tezni-bernoullijeva\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503674F6-255D-4285-8112-178FEF45A260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2BE93C-C6CA-4DCE-9770-100DED91007B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="720" windowWidth="21600" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$M$18</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$G$3:$G$52</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">(Sheet1!$L$3:$L$12,Sheet1!$N$3:$N$12)</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">(Sheet1!$N$3,Sheet1!$L$3:$L$12)</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$L$3:$L$12</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$L$4:$L$12</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$M$18</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$M$3:$M$12</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$N$3</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$N$3:$N$12</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$K$34</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$K$34</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$M$3:$M$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -180,8 +173,9 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -190,17 +184,15 @@
             <c:v>dejasnke vrednosti</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$L$3:$L$12</c:f>
@@ -279,13 +271,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1201-4AA5-A8C2-54E019674CD1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1901539232"/>
+        <c:axId val="1901537984"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -350,39 +356,39 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.9828244269951099</c:v>
+                  <c:v>0.21498663182476899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1850273479545201</c:v>
+                  <c:v>1.0171194217974999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.38441727349189</c:v>
+                  <c:v>4.2876955788961002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.50030724792044</c:v>
+                  <c:v>9.5213173875279704</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5782578001391898</c:v>
+                  <c:v>16.0453668620465</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5904699655633499</c:v>
+                  <c:v>17.3944347713479</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5498476879446699</c:v>
+                  <c:v>13.283731891689801</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.42906218183527</c:v>
+                  <c:v>5.8490113762043796</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.18244052556516</c:v>
+                  <c:v>0.99772473330512601</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.6351090630747298</c:v>
+                  <c:v>1.14008274499675E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1201-4AA5-A8C2-54E019674CD1}"/>
@@ -397,6 +403,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1901539232"/>
         <c:axId val="1901537984"/>
@@ -1446,16 +1453,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="J7" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1476,7 +1483,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1499,7 +1506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1524,26 +1531,26 @@
         <v>1</v>
       </c>
       <c r="N3">
-        <v>2.9828244269951099</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.21498663182476899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A4">
-        <f>A3+1</f>
+        <f t="shared" ref="A4:A35" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4">
         <v>0.10413699999999999</v>
       </c>
       <c r="F4">
-        <f>F3+1</f>
+        <f t="shared" ref="F4:F35" si="1">F3+1</f>
         <v>2</v>
       </c>
       <c r="G4">
         <v>0.103889</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H3:H52" si="0">2/(G4*G4)*(G$1+B$1*2-2*SQRT(B$1*B$1+B$1*G$1))</f>
+        <f t="shared" ref="H4:H52" si="2">2/(G4*G4)*(G$1+B$1*2-2*SQRT(B$1*B$1+B$1*G$1))</f>
         <v>8.5861647383605497</v>
       </c>
       <c r="L4">
@@ -1554,999 +1561,999 @@
         <v>9</v>
       </c>
       <c r="N4">
-        <v>3.1850273479545201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.0171194217974999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A5">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B5">
         <v>0.103977</v>
       </c>
       <c r="F5">
-        <f>F4+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G5">
         <v>0.10390199999999999</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5840163069779045</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L12" si="1">L4+G$57</f>
+        <f t="shared" ref="L5:L12" si="3">L4+G$57</f>
         <v>0.1039384</v>
       </c>
       <c r="M5">
         <v>7</v>
       </c>
       <c r="N5">
-        <v>3.38441727349189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>4.2876955788961002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A6">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6">
         <v>0.103909</v>
       </c>
       <c r="F6">
-        <f>F5+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="G6">
         <v>0.103909</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5828597932941673</v>
       </c>
       <c r="L6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.1039906</v>
       </c>
       <c r="M6">
         <v>6</v>
       </c>
       <c r="N6">
-        <v>3.50030724792044</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>9.5213173875279704</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A7">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7">
         <v>0.104057</v>
       </c>
       <c r="F7">
-        <f>F6+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G7">
         <v>0.10391300000000001</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5821990332660558</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.1040428</v>
       </c>
       <c r="M7">
         <v>8</v>
       </c>
       <c r="N7">
-        <v>3.5782578001391898</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>16.0453668620465</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A8">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8">
         <v>0.10392</v>
       </c>
       <c r="F8">
-        <f>F7+1</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="G8">
         <v>0.103918</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.581373190527783</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10409500000000001</v>
       </c>
       <c r="M8">
         <v>5</v>
       </c>
       <c r="N8">
-        <v>3.5904699655633499</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17.3944347713479</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A9">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B9">
         <v>0.104153</v>
       </c>
       <c r="F9">
-        <f>F8+1</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="G9">
         <v>0.10392</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5810428868090067</v>
       </c>
       <c r="L9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10414720000000001</v>
       </c>
       <c r="M9">
         <v>5</v>
       </c>
       <c r="N9">
-        <v>3.5498476879446699</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13.283731891689801</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A10">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10">
         <v>0.103922</v>
       </c>
       <c r="F10">
-        <f>F9+1</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G10">
         <v>0.103922</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5807126021603324</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10419940000000001</v>
       </c>
       <c r="M10">
         <v>6</v>
       </c>
       <c r="N10">
-        <v>3.42906218183527</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5.8490113762043796</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A11">
-        <f>A10+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B11">
         <v>0.10423399999999999</v>
       </c>
       <c r="F11">
-        <f>F10+1</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G11">
         <v>0.103926</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.580052090067424</v>
       </c>
       <c r="L11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10425160000000001</v>
       </c>
       <c r="M11">
         <v>1</v>
       </c>
       <c r="N11">
-        <v>3.18244052556516</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.99772473330512601</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A12">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B12">
         <v>0.104157</v>
       </c>
       <c r="F12">
-        <f>F11+1</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G12">
         <v>0.103934</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5787312946582599</v>
       </c>
       <c r="L12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10430380000000002</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
       <c r="N12">
-        <v>2.6351090630747298</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.14008274499675E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A13">
-        <f>A12+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B13">
         <v>0.10424899999999999</v>
       </c>
       <c r="F13">
-        <f>F12+1</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G13">
         <v>0.103949</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5762556251474553</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A14">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B14">
         <v>0.10414900000000001</v>
       </c>
       <c r="F14">
-        <f>F13+1</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G14">
         <v>0.103962</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5741109116488268</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A15">
-        <f>A14+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B15">
         <v>0.104073</v>
       </c>
       <c r="F15">
-        <f>F14+1</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="G15">
         <v>0.10396900000000001</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5729563991322735</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A16">
-        <f>A15+1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B16">
         <v>0.104224</v>
       </c>
       <c r="F16">
-        <f>F15+1</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="G16">
         <v>0.103975</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5719670025608465</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17">
-        <f>A16+1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B17">
         <v>0.104168</v>
       </c>
       <c r="F17">
-        <f>F16+1</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G17">
         <v>0.103976</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5718021197844063</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A18">
-        <f>A17+1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B18">
         <v>0.104203</v>
       </c>
       <c r="F18">
-        <f>F17+1</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="G18">
         <v>0.103977</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5716372417652256</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A19">
-        <f>A18+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B19">
         <v>0.104245</v>
       </c>
       <c r="F19">
-        <f>F18+1</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G19">
         <v>0.10399</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5694942603435909</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A20">
-        <f>A19+1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B20">
         <v>0.10399</v>
       </c>
       <c r="F20">
-        <f>F19+1</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="G20">
         <v>0.10399799999999999</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5681759019662262</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21">
-        <f>A20+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B21">
         <v>0.104029</v>
       </c>
       <c r="F21">
-        <f>F20+1</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="G21">
         <v>0.10401100000000001</v>
       </c>
       <c r="H21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5660342183785492</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A22">
-        <f>A21+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B22">
         <v>0.103962</v>
       </c>
       <c r="F22">
-        <f>F21+1</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="G22">
         <v>0.10402599999999999</v>
       </c>
       <c r="H22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5635640426638489</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23">
-        <f>A22+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B23">
         <v>0.104271</v>
       </c>
       <c r="F23">
-        <f>F22+1</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="G23">
         <v>0.104029</v>
       </c>
       <c r="H23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5630701357399612</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A24">
-        <f>A23+1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B24">
         <v>0.10402599999999999</v>
       </c>
       <c r="F24">
-        <f>F23+1</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="G24">
         <v>0.104031</v>
       </c>
       <c r="H24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5627408881955525</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A25">
-        <f>A24+1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B25">
         <v>0.104128</v>
       </c>
       <c r="F25">
-        <f>F24+1</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="G25">
         <v>0.104035</v>
       </c>
       <c r="H25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5620824500718058</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A26">
-        <f>A25+1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B26">
         <v>0.10408000000000001</v>
       </c>
       <c r="F26">
-        <f>F25+1</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="G26">
         <v>0.104056</v>
       </c>
       <c r="H26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5586268956019129</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A27">
-        <f>A26+1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B27">
         <v>0.104035</v>
       </c>
       <c r="F27">
-        <f>F26+1</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="G27">
         <v>0.104056</v>
       </c>
       <c r="H27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5586268956019129</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A28">
-        <f>A27+1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B28">
         <v>0.10406600000000001</v>
       </c>
       <c r="F28">
-        <f>F27+1</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="G28">
         <v>0.104057</v>
       </c>
       <c r="H28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5584623975715832</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A29">
-        <f>A28+1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B29">
         <v>0.104203</v>
       </c>
       <c r="F29">
-        <f>F28+1</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="G29">
         <v>0.10406600000000001</v>
       </c>
       <c r="H29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5569821286878121</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A30">
-        <f>A29+1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B30">
         <v>0.103926</v>
       </c>
       <c r="F30">
-        <f>F29+1</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="G30">
         <v>0.104073</v>
       </c>
       <c r="H30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5558310739380286</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A31">
-        <f>A30+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B31">
         <v>0.104056</v>
       </c>
       <c r="F31">
-        <f>F30+1</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="G31">
         <v>0.10408000000000001</v>
       </c>
       <c r="H31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5546802514262961</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A32">
-        <f>A31+1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B32">
         <v>0.10435</v>
       </c>
       <c r="F32">
-        <f>F31+1</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="G32">
         <v>0.104084</v>
       </c>
       <c r="H32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5540227428085576</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A33">
-        <f>A32+1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B33">
         <v>0.103918</v>
       </c>
       <c r="F33">
-        <f>F32+1</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="G33">
         <v>0.104089</v>
       </c>
       <c r="H33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.553200963629866</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A34">
-        <f>A33+1</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B34">
         <v>0.103834</v>
       </c>
       <c r="F34">
-        <f>F33+1</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="G34">
         <v>0.10409599999999999</v>
       </c>
       <c r="H34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5520506717134275</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A35">
-        <f>A34+1</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B35">
         <v>0.103949</v>
       </c>
       <c r="F35">
-        <f>F34+1</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="G35">
         <v>0.104101</v>
       </c>
       <c r="H35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5512291766948358</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A36">
-        <f>A35+1</f>
+        <f t="shared" ref="A36:A52" si="4">A35+1</f>
         <v>34</v>
       </c>
       <c r="B36">
         <v>0.103934</v>
       </c>
       <c r="F36">
-        <f>F35+1</f>
+        <f t="shared" ref="F36:F52" si="5">F35+1</f>
         <v>34</v>
       </c>
       <c r="G36">
         <v>0.104128</v>
       </c>
       <c r="H36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5467951483028912</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A37">
-        <f>A36+1</f>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="B37">
         <v>0.10409599999999999</v>
       </c>
       <c r="F37">
-        <f>F36+1</f>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="G37">
         <v>0.10413699999999999</v>
       </c>
       <c r="H37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.54531790520209</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A38">
-        <f>A37+1</f>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="B38">
         <v>0.104144</v>
       </c>
       <c r="F38">
-        <f>F37+1</f>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="G38">
         <v>0.104144</v>
       </c>
       <c r="H38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.544169203115743</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A39">
-        <f>A38+1</f>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="B39">
         <v>0.104031</v>
       </c>
       <c r="F39">
-        <f>F38+1</f>
+        <f t="shared" si="5"/>
         <v>37</v>
       </c>
       <c r="G39">
         <v>0.10414900000000001</v>
       </c>
       <c r="H39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.543348843428344</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A40">
-        <f>A39+1</f>
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
       <c r="B40">
         <v>0.104356</v>
       </c>
       <c r="F40">
-        <f>F39+1</f>
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="G40">
         <v>0.104153</v>
       </c>
       <c r="H40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5426926407427111</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A41">
-        <f>A40+1</f>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
       <c r="B41">
         <v>0.104101</v>
       </c>
       <c r="F41">
-        <f>F40+1</f>
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="G41">
         <v>0.104157</v>
       </c>
       <c r="H41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5420365136571892</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A42">
-        <f>A41+1</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="B42">
         <v>0.103976</v>
       </c>
       <c r="F42">
-        <f>F41+1</f>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="G42">
         <v>0.104168</v>
       </c>
       <c r="H42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5402325538902968</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A43">
-        <f>A42+1</f>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="B43">
         <v>0.10417899999999999</v>
       </c>
       <c r="F43">
-        <f>F42+1</f>
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="G43">
         <v>0.10417899999999999</v>
       </c>
       <c r="H43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5384291655200322</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A44">
-        <f>A43+1</f>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="B44">
         <v>0.103889</v>
       </c>
       <c r="F44">
-        <f>F43+1</f>
+        <f t="shared" si="5"/>
         <v>42</v>
       </c>
       <c r="G44">
         <v>0.104203</v>
       </c>
       <c r="H44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5344964821778078</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A45">
-        <f>A44+1</f>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="B45">
         <v>0.104089</v>
       </c>
       <c r="F45">
-        <f>F44+1</f>
+        <f t="shared" si="5"/>
         <v>43</v>
       </c>
       <c r="G45">
         <v>0.104203</v>
       </c>
       <c r="H45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5344964821778078</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A46">
-        <f>A45+1</f>
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
       <c r="B46">
         <v>0.10391300000000001</v>
       </c>
       <c r="F46">
-        <f>F45+1</f>
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="G46">
         <v>0.104224</v>
       </c>
       <c r="H46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5310576126229734</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A47">
-        <f>A46+1</f>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="B47">
         <v>0.10396900000000001</v>
       </c>
       <c r="F47">
-        <f>F46+1</f>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="G47">
         <v>0.10423399999999999</v>
       </c>
       <c r="H47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5294207861774041</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A48">
-        <f>A47+1</f>
+        <f t="shared" si="4"/>
         <v>46</v>
       </c>
       <c r="B48">
         <v>0.104084</v>
       </c>
       <c r="F48">
-        <f>F47+1</f>
+        <f t="shared" si="5"/>
         <v>46</v>
       </c>
       <c r="G48">
         <v>0.104245</v>
       </c>
       <c r="H48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5276208211242519</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A49">
-        <f>A48+1</f>
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
       <c r="B49">
         <v>0.10399799999999999</v>
       </c>
       <c r="F49">
-        <f>F48+1</f>
+        <f t="shared" si="5"/>
         <v>47</v>
       </c>
       <c r="G49">
         <v>0.10424899999999999</v>
       </c>
       <c r="H49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5269664296407761</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A50">
-        <f>A49+1</f>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="B50">
         <v>0.10401100000000001</v>
       </c>
       <c r="F50">
-        <f>F49+1</f>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="G50">
@@ -2557,47 +2564,47 @@
         <v>8.5233686225529866</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A51">
-        <f>A50+1</f>
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
       <c r="B51">
         <v>0.104056</v>
       </c>
       <c r="F51">
-        <f>F50+1</f>
+        <f t="shared" si="5"/>
         <v>49</v>
       </c>
       <c r="G51">
         <v>0.10435</v>
       </c>
       <c r="H51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5104679759419888</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A52">
-        <f>A51+1</f>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="B52">
         <v>0.10390199999999999</v>
       </c>
       <c r="F52">
-        <f>F51+1</f>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
       <c r="G52">
         <v>0.104356</v>
       </c>
       <c r="H52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5094893769172089</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.5">
       <c r="F53" t="s">
         <v>2</v>
       </c>
@@ -2614,7 +2621,7 @@
         <v>2.7861148966338159E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.5">
       <c r="F54" t="s">
         <v>5</v>
       </c>
@@ -2623,7 +2630,7 @@
         <v>0.103834</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.5">
       <c r="F55" t="s">
         <v>6</v>
       </c>
@@ -2632,7 +2639,7 @@
         <v>0.104356</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.5">
       <c r="F56" t="s">
         <v>7</v>
       </c>
@@ -2641,7 +2648,7 @@
         <v>5.2200000000000857E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.5">
       <c r="F57" t="s">
         <v>8</v>
       </c>
@@ -2650,7 +2657,7 @@
         <v>5.2200000000000855E-5</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.5">
       <c r="F59" t="s">
         <v>9</v>
       </c>
@@ -2667,7 +2674,7 @@
         <v>7.2001886884152225E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.5">
       <c r="F62" t="s">
         <v>10</v>
       </c>
@@ -2676,7 +2683,7 @@
         <v>8.5355339059327382E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.5">
       <c r="G63" t="s">
         <v>13</v>
       </c>
@@ -2687,7 +2694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.5">
       <c r="F64" t="s">
         <v>11</v>
       </c>
@@ -2704,7 +2711,7 @@
         <v>6.921577198751841E-2</v>
       </c>
     </row>
-    <row r="65" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:9" x14ac:dyDescent="0.5">
       <c r="F65" t="s">
         <v>12</v>
       </c>
@@ -2721,7 +2728,7 @@
         <v>2.7861148966338159E-3</v>
       </c>
     </row>
-    <row r="66" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:9" x14ac:dyDescent="0.5">
       <c r="H66" t="s">
         <v>16</v>
       </c>

</xml_diff>